<commit_message>
updated ie test results
</commit_message>
<xml_diff>
--- a/ie_test-results.xlsx
+++ b/ie_test-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\anu\comp4450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AED81F-5A44-4CEE-8669-BF16058A0563}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E792AB-6435-4E85-A6C8-8C826343BDB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E9B88CD1-3B0D-4A75-AE61-841D3335B013}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>bert</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>Mean</t>
+  </si>
+  <si>
+    <t>gkr</t>
+  </si>
+  <si>
+    <t>hy-nli</t>
+  </si>
+  <si>
+    <t>523a</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>614a</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>623a</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>1958a</t>
   </si>
 </sst>
 </file>
@@ -72,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -80,12 +107,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2321462-3F7F-4639-8933-79D80AEC3C8E}">
-  <dimension ref="A1:AR7"/>
+  <dimension ref="A1:AR54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AM13" sqref="AM13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,6 +508,7 @@
     <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
@@ -789,6 +887,1093 @@
         <v>0.84470684039087929</v>
       </c>
     </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.71230896323833104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0.71045022717885098</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.70095002065262202</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.70198265179677799</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.67699297810821901</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.69971086327963605</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.71334159438248601</v>
+      </c>
+      <c r="I12">
+        <f>AVERAGE(D12:H12)</f>
+        <v>0.69859562164394828</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.70033044196612904</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.70342833539859495</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0.70280875671210197</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0.70735233374638495</v>
+      </c>
+      <c r="O12" s="6">
+        <v>0.69062370921106897</v>
+      </c>
+      <c r="P12">
+        <f>AVERAGE(K12:O12)</f>
+        <v>0.70090871540685595</v>
+      </c>
+      <c r="R12" s="6">
+        <v>0.70384138785625705</v>
+      </c>
+      <c r="S12" s="6">
+        <v>0.69909128459314296</v>
+      </c>
+      <c r="T12" s="6">
+        <v>0.69950433705080495</v>
+      </c>
+      <c r="U12" s="6">
+        <v>0.71024370095001998</v>
+      </c>
+      <c r="V12" s="6">
+        <v>0.70384138785625705</v>
+      </c>
+      <c r="W12">
+        <f>AVERAGE(R12:V12)</f>
+        <v>0.70330441966129642</v>
+      </c>
+      <c r="Y12" s="6">
+        <v>0.693515076414704</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>0.69991738950846705</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>0.70074349442379102</v>
+      </c>
+      <c r="AB12" s="6">
+        <v>0.70033044196612904</v>
+      </c>
+      <c r="AC12" s="6">
+        <v>0.70404791408508804</v>
+      </c>
+      <c r="AD12">
+        <f>AVERAGE(Y12:AC12)</f>
+        <v>0.69971086327963583</v>
+      </c>
+      <c r="AF12" s="6">
+        <v>0.69599339116067704</v>
+      </c>
+      <c r="AG12" s="6">
+        <v>0.705493597686906</v>
+      </c>
+      <c r="AH12" s="6">
+        <v>0.69392812887236599</v>
+      </c>
+      <c r="AI12" s="6">
+        <v>0.70838496489054104</v>
+      </c>
+      <c r="AJ12" s="6">
+        <v>0.70652622883106098</v>
+      </c>
+      <c r="AK12">
+        <f>AVERAGE(AF12:AJ12)</f>
+        <v>0.70206526228831023</v>
+      </c>
+      <c r="AM12" s="6">
+        <v>0.69661296984717003</v>
+      </c>
+      <c r="AN12" s="6">
+        <v>0.69785212722015699</v>
+      </c>
+      <c r="AO12" s="6">
+        <v>0.68835192069392803</v>
+      </c>
+      <c r="AP12" s="6">
+        <v>0.69434118133002798</v>
+      </c>
+      <c r="AQ12" s="6">
+        <v>0.69578686493184605</v>
+      </c>
+      <c r="AR12">
+        <f>AVERAGE(AM12:AQ12)</f>
+        <v>0.69458901280462582</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.66383595691797803</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.66280033140016503</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.62696768848384399</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.66487158243579103</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.67833471416735702</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(D13:H13)</f>
+        <v>0.65936205468102693</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.68061309030654504</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0.685376967688483</v>
+      </c>
+      <c r="M13" s="6">
+        <v>0.69014084507042195</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0.68496271748135795</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0.66735708367854096</v>
+      </c>
+      <c r="P13">
+        <f>AVERAGE(K13:O13)</f>
+        <v>0.68169014084506974</v>
+      </c>
+      <c r="R13" s="6">
+        <v>0.68102734051366998</v>
+      </c>
+      <c r="S13" s="6">
+        <v>0.681234465617232</v>
+      </c>
+      <c r="T13" s="6">
+        <v>0.67957746478873204</v>
+      </c>
+      <c r="U13" s="6">
+        <v>0.68951946975973399</v>
+      </c>
+      <c r="V13" s="6">
+        <v>0.67978458989229495</v>
+      </c>
+      <c r="W13">
+        <f>AVERAGE(R13:V13)</f>
+        <v>0.68222866611433253</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>0.68019884009942</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>0.68682684341342104</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>0.68206296603148298</v>
+      </c>
+      <c r="AB13" s="6">
+        <v>0.686412593206296</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>0.68703396851698395</v>
+      </c>
+      <c r="AD13">
+        <f>AVERAGE(Y13:AC13)</f>
+        <v>0.68450704225352077</v>
+      </c>
+      <c r="AF13" s="6">
+        <v>0.68040596520298202</v>
+      </c>
+      <c r="AG13" s="6">
+        <v>0.68703396851698395</v>
+      </c>
+      <c r="AH13" s="6">
+        <v>0.68454846727423302</v>
+      </c>
+      <c r="AI13" s="6">
+        <v>0.69159072079535999</v>
+      </c>
+      <c r="AJ13" s="6">
+        <v>0.69241922120960997</v>
+      </c>
+      <c r="AK13">
+        <f>AVERAGE(AF13:AJ13)</f>
+        <v>0.68719966859983372</v>
+      </c>
+      <c r="AM13" s="6">
+        <v>0.68661971830985902</v>
+      </c>
+      <c r="AN13" s="6">
+        <v>0.68164871582435704</v>
+      </c>
+      <c r="AO13" s="6">
+        <v>0.67833471416735702</v>
+      </c>
+      <c r="AP13" s="6">
+        <v>0.68786246893123404</v>
+      </c>
+      <c r="AQ13" s="6">
+        <v>0.683305716652858</v>
+      </c>
+      <c r="AR13">
+        <f>AVERAGE(AM13:AQ13)</f>
+        <v>0.68355426677713305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="S17" s="6"/>
+    </row>
+    <row r="18" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="5:32" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.70095002065262202</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0.66383595691797803</v>
+      </c>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.70198265179677799</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0</v>
+      </c>
+      <c r="M25" s="5">
+        <v>1</v>
+      </c>
+      <c r="N25" s="5">
+        <v>0.66280033140016503</v>
+      </c>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="U25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W25" s="1">
+        <v>1</v>
+      </c>
+      <c r="X25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>2</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.67699297810821901</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0</v>
+      </c>
+      <c r="M26" s="5">
+        <v>2</v>
+      </c>
+      <c r="N26" s="5">
+        <v>0.62696768848384399</v>
+      </c>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="U26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W26" s="1">
+        <v>0</v>
+      </c>
+      <c r="X26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>3</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.69971086327963605</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0</v>
+      </c>
+      <c r="M27" s="5">
+        <v>3</v>
+      </c>
+      <c r="N27" s="5">
+        <v>0.66487158243579103</v>
+      </c>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="U27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W27" s="1">
+        <v>1</v>
+      </c>
+      <c r="X27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>4</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.71334159438248601</v>
+      </c>
+      <c r="L28" s="4">
+        <v>0</v>
+      </c>
+      <c r="M28" s="5">
+        <v>4</v>
+      </c>
+      <c r="N28" s="5">
+        <v>0.67833471416735702</v>
+      </c>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="U28" t="s">
+        <v>13</v>
+      </c>
+      <c r="V28" t="s">
+        <v>8</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+      <c r="AD28">
+        <v>0</v>
+      </c>
+      <c r="AE28">
+        <v>0</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E29" s="4">
+        <v>20</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.70033044196612904</v>
+      </c>
+      <c r="L29" s="4">
+        <v>20</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+      <c r="N29" s="5">
+        <v>0.68061309030654504</v>
+      </c>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="4">
+        <v>20</v>
+      </c>
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.70342833539859495</v>
+      </c>
+      <c r="L30" s="4">
+        <v>20</v>
+      </c>
+      <c r="M30" s="5">
+        <v>1</v>
+      </c>
+      <c r="N30" s="5">
+        <v>0.685376967688483</v>
+      </c>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+    </row>
+    <row r="31" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E31" s="4">
+        <v>20</v>
+      </c>
+      <c r="F31" s="5">
+        <v>2</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.70280875671210197</v>
+      </c>
+      <c r="L31" s="4">
+        <v>20</v>
+      </c>
+      <c r="M31" s="5">
+        <v>2</v>
+      </c>
+      <c r="N31" s="5">
+        <v>0.69014084507042195</v>
+      </c>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="5:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="4">
+        <v>20</v>
+      </c>
+      <c r="F32" s="5">
+        <v>3</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.70735233374638495</v>
+      </c>
+      <c r="L32" s="4">
+        <v>20</v>
+      </c>
+      <c r="M32" s="5">
+        <v>3</v>
+      </c>
+      <c r="N32" s="5">
+        <v>0.68496271748135795</v>
+      </c>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+    </row>
+    <row r="33" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E33" s="4">
+        <v>20</v>
+      </c>
+      <c r="F33" s="5">
+        <v>4</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.69062370921106897</v>
+      </c>
+      <c r="L33" s="4">
+        <v>20</v>
+      </c>
+      <c r="M33" s="5">
+        <v>4</v>
+      </c>
+      <c r="N33" s="5">
+        <v>0.66735708367854096</v>
+      </c>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+    </row>
+    <row r="34" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E34" s="4">
+        <v>40</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.70384138785625705</v>
+      </c>
+      <c r="L34" s="4">
+        <v>40</v>
+      </c>
+      <c r="M34" s="5">
+        <v>0</v>
+      </c>
+      <c r="N34" s="5">
+        <v>0.68102734051366998</v>
+      </c>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+    </row>
+    <row r="35" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E35" s="4">
+        <v>40</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0.69909128459314296</v>
+      </c>
+      <c r="L35" s="4">
+        <v>40</v>
+      </c>
+      <c r="M35" s="5">
+        <v>1</v>
+      </c>
+      <c r="N35" s="5">
+        <v>0.681234465617232</v>
+      </c>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+    </row>
+    <row r="36" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E36" s="4">
+        <v>40</v>
+      </c>
+      <c r="F36" s="5">
+        <v>2</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0.69950433705080495</v>
+      </c>
+      <c r="L36" s="4">
+        <v>40</v>
+      </c>
+      <c r="M36" s="5">
+        <v>2</v>
+      </c>
+      <c r="N36" s="5">
+        <v>0.67957746478873204</v>
+      </c>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+    </row>
+    <row r="37" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E37" s="4">
+        <v>40</v>
+      </c>
+      <c r="F37" s="5">
+        <v>3</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0.71024370095001998</v>
+      </c>
+      <c r="L37" s="4">
+        <v>40</v>
+      </c>
+      <c r="M37" s="5">
+        <v>3</v>
+      </c>
+      <c r="N37" s="5">
+        <v>0.68951946975973399</v>
+      </c>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+    </row>
+    <row r="38" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E38" s="4">
+        <v>40</v>
+      </c>
+      <c r="F38" s="5">
+        <v>4</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0.70384138785625705</v>
+      </c>
+      <c r="L38" s="4">
+        <v>40</v>
+      </c>
+      <c r="M38" s="5">
+        <v>4</v>
+      </c>
+      <c r="N38" s="5">
+        <v>0.67978458989229495</v>
+      </c>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+    </row>
+    <row r="39" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E39" s="4">
+        <v>60</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0.693515076414704</v>
+      </c>
+      <c r="L39" s="4">
+        <v>60</v>
+      </c>
+      <c r="M39" s="5">
+        <v>0</v>
+      </c>
+      <c r="N39" s="5">
+        <v>0.68019884009942</v>
+      </c>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+    </row>
+    <row r="40" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E40" s="4">
+        <v>60</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.69991738950846705</v>
+      </c>
+      <c r="L40" s="4">
+        <v>60</v>
+      </c>
+      <c r="M40" s="5">
+        <v>1</v>
+      </c>
+      <c r="N40" s="5">
+        <v>0.68682684341342104</v>
+      </c>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+    </row>
+    <row r="41" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E41" s="4">
+        <v>60</v>
+      </c>
+      <c r="F41" s="5">
+        <v>2</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0.70074349442379102</v>
+      </c>
+      <c r="L41" s="4">
+        <v>60</v>
+      </c>
+      <c r="M41" s="5">
+        <v>2</v>
+      </c>
+      <c r="N41" s="5">
+        <v>0.68206296603148298</v>
+      </c>
+      <c r="R41" s="6"/>
+    </row>
+    <row r="42" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E42" s="4">
+        <v>60</v>
+      </c>
+      <c r="F42" s="5">
+        <v>3</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0.70033044196612904</v>
+      </c>
+      <c r="L42" s="4">
+        <v>60</v>
+      </c>
+      <c r="M42" s="5">
+        <v>3</v>
+      </c>
+      <c r="N42" s="5">
+        <v>0.686412593206296</v>
+      </c>
+      <c r="R42" s="6"/>
+    </row>
+    <row r="43" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E43" s="4">
+        <v>60</v>
+      </c>
+      <c r="F43" s="5">
+        <v>4</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0.70404791408508804</v>
+      </c>
+      <c r="L43" s="4">
+        <v>60</v>
+      </c>
+      <c r="M43" s="5">
+        <v>4</v>
+      </c>
+      <c r="N43" s="5">
+        <v>0.68703396851698395</v>
+      </c>
+      <c r="R43" s="6"/>
+    </row>
+    <row r="44" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E44" s="4">
+        <v>80</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0.69599339116067704</v>
+      </c>
+      <c r="L44" s="4">
+        <v>80</v>
+      </c>
+      <c r="M44" s="5">
+        <v>0</v>
+      </c>
+      <c r="N44" s="5">
+        <v>0.68040596520298202</v>
+      </c>
+      <c r="R44" s="6"/>
+    </row>
+    <row r="45" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E45" s="4">
+        <v>80</v>
+      </c>
+      <c r="F45" s="5">
+        <v>1</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0.705493597686906</v>
+      </c>
+      <c r="L45" s="4">
+        <v>80</v>
+      </c>
+      <c r="M45" s="5">
+        <v>1</v>
+      </c>
+      <c r="N45" s="5">
+        <v>0.68703396851698395</v>
+      </c>
+      <c r="R45" s="6"/>
+    </row>
+    <row r="46" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E46" s="4">
+        <v>80</v>
+      </c>
+      <c r="F46" s="5">
+        <v>2</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0.69392812887236599</v>
+      </c>
+      <c r="L46" s="4">
+        <v>80</v>
+      </c>
+      <c r="M46" s="5">
+        <v>2</v>
+      </c>
+      <c r="N46" s="5">
+        <v>0.68454846727423302</v>
+      </c>
+      <c r="R46" s="6"/>
+    </row>
+    <row r="47" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E47" s="4">
+        <v>80</v>
+      </c>
+      <c r="F47" s="5">
+        <v>3</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0.70838496489054104</v>
+      </c>
+      <c r="L47" s="4">
+        <v>80</v>
+      </c>
+      <c r="M47" s="5">
+        <v>3</v>
+      </c>
+      <c r="N47" s="5">
+        <v>0.69159072079535999</v>
+      </c>
+      <c r="R47" s="6"/>
+    </row>
+    <row r="48" spans="5:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E48" s="4">
+        <v>80</v>
+      </c>
+      <c r="F48" s="5">
+        <v>4</v>
+      </c>
+      <c r="G48" s="5">
+        <v>0.70652622883106098</v>
+      </c>
+      <c r="L48" s="4">
+        <v>80</v>
+      </c>
+      <c r="M48" s="5">
+        <v>4</v>
+      </c>
+      <c r="N48" s="5">
+        <v>0.69241922120960997</v>
+      </c>
+      <c r="R48" s="6"/>
+    </row>
+    <row r="49" spans="5:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E49" s="4">
+        <v>100</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0</v>
+      </c>
+      <c r="G49" s="5">
+        <v>0.69661296984717003</v>
+      </c>
+      <c r="L49" s="4">
+        <v>100</v>
+      </c>
+      <c r="M49" s="5">
+        <v>0</v>
+      </c>
+      <c r="N49" s="5">
+        <v>0.68661971830985902</v>
+      </c>
+      <c r="R49" s="6"/>
+    </row>
+    <row r="50" spans="5:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E50" s="4">
+        <v>100</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1</v>
+      </c>
+      <c r="G50" s="5">
+        <v>0.69785212722015699</v>
+      </c>
+      <c r="L50" s="4">
+        <v>100</v>
+      </c>
+      <c r="M50" s="5">
+        <v>1</v>
+      </c>
+      <c r="N50" s="5">
+        <v>0.68164871582435704</v>
+      </c>
+    </row>
+    <row r="51" spans="5:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E51" s="4">
+        <v>100</v>
+      </c>
+      <c r="F51" s="5">
+        <v>2</v>
+      </c>
+      <c r="G51" s="5">
+        <v>0.68835192069392803</v>
+      </c>
+      <c r="L51" s="4">
+        <v>100</v>
+      </c>
+      <c r="M51" s="5">
+        <v>2</v>
+      </c>
+      <c r="N51" s="5">
+        <v>0.67833471416735702</v>
+      </c>
+    </row>
+    <row r="52" spans="5:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E52" s="4">
+        <v>100</v>
+      </c>
+      <c r="F52" s="5">
+        <v>3</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0.69434118133002798</v>
+      </c>
+      <c r="L52" s="4">
+        <v>100</v>
+      </c>
+      <c r="M52" s="5">
+        <v>3</v>
+      </c>
+      <c r="N52" s="5">
+        <v>0.68786246893123404</v>
+      </c>
+    </row>
+    <row r="53" spans="5:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E53" s="4">
+        <v>100</v>
+      </c>
+      <c r="F53" s="5">
+        <v>4</v>
+      </c>
+      <c r="G53" s="5">
+        <v>0.69578686493184605</v>
+      </c>
+      <c r="L53" s="4">
+        <v>100</v>
+      </c>
+      <c r="M53" s="5">
+        <v>4</v>
+      </c>
+      <c r="N53" s="5">
+        <v>0.683305716652858</v>
+      </c>
+    </row>
+    <row r="54" spans="5:18" x14ac:dyDescent="0.3">
+      <c r="E54" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>